<commit_message>
updated user data excel sheet updated
</commit_message>
<xml_diff>
--- a/src/main/resources/batch/students_data.xlsx
+++ b/src/main/resources/batch/students_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>FirstName</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>a9874589745</t>
+  </si>
+  <si>
+    <t>GenderId</t>
+  </si>
+  <si>
+    <t>CasteId</t>
+  </si>
+  <si>
+    <t>ReligionId</t>
+  </si>
+  <si>
+    <t>IdProof</t>
   </si>
 </sst>
 </file>
@@ -514,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,9 +548,12 @@
     <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.140625" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" customWidth="1"/>
+    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,8 +623,20 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -641,7 +668,7 @@
         <v>29</v>
       </c>
       <c r="K2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L2">
         <v>37</v>
@@ -679,8 +706,20 @@
       <c r="W2">
         <v>535501</v>
       </c>
+      <c r="X2">
+        <v>30</v>
+      </c>
+      <c r="Y2">
+        <v>37</v>
+      </c>
+      <c r="Z2">
+        <v>41</v>
+      </c>
+      <c r="AA2">
+        <v>1345678970</v>
+      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -712,7 +751,7 @@
         <v>29</v>
       </c>
       <c r="K3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L3">
         <v>38</v>
@@ -750,8 +789,20 @@
       <c r="W3">
         <v>535501</v>
       </c>
+      <c r="X3">
+        <v>31</v>
+      </c>
+      <c r="Y3">
+        <v>37</v>
+      </c>
+      <c r="Z3">
+        <v>41</v>
+      </c>
+      <c r="AA3">
+        <v>12345678998</v>
+      </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -783,7 +834,7 @@
         <v>29</v>
       </c>
       <c r="K4">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L4">
         <v>40</v>
@@ -820,6 +871,18 @@
       </c>
       <c r="W4">
         <v>535501</v>
+      </c>
+      <c r="X4">
+        <v>30</v>
+      </c>
+      <c r="Y4">
+        <v>37</v>
+      </c>
+      <c r="Z4">
+        <v>41</v>
+      </c>
+      <c r="AA4">
+        <v>1234547822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>